<commit_message>
data change done for production run.
</commit_message>
<xml_diff>
--- a/QA_Automation/Invessence/TestCases/PROD/TestData_Invessence_PROD_OpenNewAccount.xlsx
+++ b/QA_Automation/Invessence/TestCases/PROD/TestData_Invessence_PROD_OpenNewAccount.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="126">
   <si>
     <t>TCID</t>
   </si>
@@ -58,9 +58,6 @@
     <t>TC002</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>Investing amount limits $2000 to ?</t>
   </si>
   <si>
@@ -274,12 +271,6 @@
     <t>25000</t>
   </si>
   <si>
-    <t>Joint</t>
-  </si>
-  <si>
-    <t>UTMA / UGMA</t>
-  </si>
-  <si>
     <t>TC003</t>
   </si>
   <si>
@@ -319,96 +310,21 @@
     <t>BuildingBenjamins-identity.png</t>
   </si>
   <si>
-    <t>25001</t>
-  </si>
-  <si>
-    <t>25002</t>
-  </si>
-  <si>
-    <t>25003</t>
-  </si>
-  <si>
-    <t>TC004</t>
-  </si>
-  <si>
-    <t>ACAT</t>
-  </si>
-  <si>
-    <t>street2</t>
-  </si>
-  <si>
-    <t>city2</t>
-  </si>
-  <si>
-    <t>street3</t>
-  </si>
-  <si>
-    <t>city3</t>
-  </si>
-  <si>
-    <t>street4</t>
-  </si>
-  <si>
-    <t>city4</t>
-  </si>
-  <si>
     <t>ABC1</t>
   </si>
   <si>
-    <t>ABC2</t>
-  </si>
-  <si>
-    <t>ABC3</t>
-  </si>
-  <si>
-    <t>ABC4</t>
-  </si>
-  <si>
     <t>BenificiaryFN1</t>
   </si>
   <si>
-    <t>BenificiaryFN2</t>
-  </si>
-  <si>
-    <t>BenificiaryFN3</t>
-  </si>
-  <si>
-    <t>BenificiaryFN4</t>
-  </si>
-  <si>
     <t>BenificiarylN1</t>
   </si>
   <si>
-    <t>BenificiarylN2</t>
-  </si>
-  <si>
-    <t>BenificiarylN3</t>
-  </si>
-  <si>
-    <t>BenificiarylN4</t>
-  </si>
-  <si>
     <t>Test bank1</t>
   </si>
   <si>
-    <t>Test bank2</t>
-  </si>
-  <si>
-    <t>Test bank3</t>
-  </si>
-  <si>
-    <t>Test bank4</t>
-  </si>
-  <si>
     <t>testfirm1</t>
   </si>
   <si>
-    <t>testfirm2</t>
-  </si>
-  <si>
-    <t>testfirm3</t>
-  </si>
-  <si>
     <t>2501</t>
   </si>
   <si>
@@ -418,46 +334,70 @@
     <t>2503</t>
   </si>
   <si>
-    <t>2504</t>
-  </si>
-  <si>
-    <t>OptionsXpress, Inc.</t>
-  </si>
-  <si>
     <t>04/05/2017</t>
   </si>
   <si>
     <t>bbqa.user</t>
   </si>
   <si>
-    <t>http://uatbb.invessence.com:8080//login.xhtml</t>
-  </si>
-  <si>
     <t>BB-testfname1</t>
   </si>
   <si>
     <t>BB-testlname1</t>
   </si>
   <si>
-    <t>BB-testfname2</t>
-  </si>
-  <si>
-    <t>BB-testfname3</t>
-  </si>
-  <si>
-    <t>BB-testfname4</t>
-  </si>
-  <si>
-    <t>BB-testlname2</t>
-  </si>
-  <si>
-    <t>BB-testlname3</t>
-  </si>
-  <si>
-    <t>BB-testlname4</t>
-  </si>
-  <si>
     <t>https://www.buildingbenjamins.com/login.xhtml</t>
+  </si>
+  <si>
+    <t>http://uattcm.invessence.com:8080//login.xhtml?rep=100</t>
+  </si>
+  <si>
+    <t>tcmintrepqa.user</t>
+  </si>
+  <si>
+    <t>tcm100testfname1</t>
+  </si>
+  <si>
+    <t>tcm100testlname1</t>
+  </si>
+  <si>
+    <t>05/04/2017</t>
+  </si>
+  <si>
+    <t>tcm-logo.jpe</t>
+  </si>
+  <si>
+    <t>http://uattcm.invessence.com:8080/login.xhtml?rep=200</t>
+  </si>
+  <si>
+    <t>tcmextrepqa.user</t>
+  </si>
+  <si>
+    <t>25018</t>
+  </si>
+  <si>
+    <t>tcm200testfname1</t>
+  </si>
+  <si>
+    <t>tcm200testlname1</t>
+  </si>
+  <si>
+    <t>BenificiaryFNRep200</t>
+  </si>
+  <si>
+    <t>BenificiaryFNRep100</t>
+  </si>
+  <si>
+    <t>BenificiarylNRep100</t>
+  </si>
+  <si>
+    <t>BenificiarylNRep200</t>
+  </si>
+  <si>
+    <t>Test bankRep200</t>
+  </si>
+  <si>
+    <t>Test bankRep100</t>
   </si>
 </sst>
 </file>
@@ -502,7 +442,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -514,6 +454,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -833,12 +776,12 @@
   <dimension ref="A1:BD5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="BC6" sqref="BC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="45" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
@@ -850,11 +793,16 @@
     <col min="11" max="11" width="25.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.85546875" style="3" customWidth="1"/>
     <col min="13" max="13" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="18" width="13.85546875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="13.85546875" style="3" customWidth="1"/>
     <col min="19" max="19" width="33.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="20" max="23" width="13.85546875" style="3" customWidth="1"/>
     <col min="24" max="24" width="23.42578125" style="3" customWidth="1"/>
-    <col min="25" max="38" width="13.85546875" style="3" customWidth="1"/>
+    <col min="25" max="28" width="13.85546875" style="3" customWidth="1"/>
+    <col min="29" max="29" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="38" width="13.85546875" style="3" customWidth="1"/>
     <col min="39" max="39" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="40" max="45" width="13.85546875" style="3" customWidth="1"/>
     <col min="46" max="46" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
@@ -879,151 +827,151 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="M1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AS1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AT1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AU1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AR1" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="AS1" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AV1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AW1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AY1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AZ1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BA1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="BB1" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="AU1" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AV1" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AW1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AX1" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="AY1" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="AZ1" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="BA1" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="BB1" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="BC1" t="s">
         <v>8</v>
@@ -1037,164 +985,164 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>145</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>129</v>
+        <v>101</v>
       </c>
       <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="K2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>137</v>
+        <v>106</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>138</v>
+        <v>107</v>
       </c>
       <c r="P2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="T2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="S2" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="T2" s="4" t="s">
+      <c r="U2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="V2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="W2" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="X2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="Y2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="AA2" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC2" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AE2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG2" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="AA2" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC2" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="AD2" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="AE2" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AH2" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AI2" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="AJ2" s="4" t="s">
+      <c r="AK2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="AK2" s="4" t="s">
+      <c r="AL2" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AL2" s="4" t="s">
+      <c r="AM2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AN2" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="AM2" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="AN2" s="4" t="s">
+      <c r="AO2" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="AO2" s="4" t="s">
+      <c r="AP2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="AP2" s="4" t="s">
+      <c r="AQ2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="AQ2" s="4" t="s">
+      <c r="AR2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AT2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AU2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="AR2" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="AS2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AT2" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="AU2" s="4" t="s">
+      <c r="AV2" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="AV2" s="4" t="s">
-        <v>83</v>
-      </c>
       <c r="AW2" s="4" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="AX2" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AY2" s="4"/>
       <c r="AZ2" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="BA2" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="BB2" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="BC2" s="6" t="s">
-        <v>12</v>
+        <v>95</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>9</v>
       </c>
       <c r="BD2" s="2"/>
     </row>
@@ -1203,314 +1151,318 @@
         <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>136</v>
+        <v>109</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
-        <v>135</v>
+      <c r="D3" s="8" t="s">
+        <v>110</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="K3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="S3" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="P3" s="4" t="s">
+      <c r="T3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC3" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD3" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="AE3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF3" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="Q3" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="U3" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="V3" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="W3" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="X3" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y3" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z3" s="4" t="s">
+      <c r="AG3" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="AA3" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="AB3" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC3" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="AD3" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="AE3" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF3" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG3" s="4" t="s">
+      <c r="AH3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="AH3" s="4" t="s">
+      <c r="AI3" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="AI3" s="4" t="s">
+      <c r="AJ3" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="AJ3" s="4" t="s">
+      <c r="AK3" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="AK3" s="4" t="s">
+      <c r="AL3" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AL3" s="4" t="s">
+      <c r="AM3" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="AN3" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="AM3" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="AN3" s="4" t="s">
+      <c r="AO3" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="AO3" s="4" t="s">
+      <c r="AP3" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="AP3" s="4" t="s">
+      <c r="AQ3" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="AQ3" s="4" t="s">
+      <c r="AR3" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AT3" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AU3" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="AR3" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="AS3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AT3" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU3" s="4" t="s">
+      <c r="AV3" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="AV3" s="4" t="s">
-        <v>99</v>
-      </c>
       <c r="AW3" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="AX3" s="4"/>
+        <v>113</v>
+      </c>
+      <c r="AX3" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="AY3" s="4"/>
       <c r="AZ3" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="BA3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="BB3" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="BC3" s="6" t="s">
-        <v>12</v>
+        <v>114</v>
+      </c>
+      <c r="BC3" t="s">
+        <v>9</v>
       </c>
       <c r="BD3" s="2"/>
     </row>
     <row r="4" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
-        <v>135</v>
+      <c r="D4" s="8" t="s">
+        <v>116</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>131</v>
+        <v>103</v>
       </c>
       <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="K4" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>85</v>
+        <v>27</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="P4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q4" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="S4" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="T4" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="S4" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>106</v>
-      </c>
       <c r="U4" s="4" t="s">
-        <v>107</v>
+        <v>65</v>
       </c>
       <c r="V4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="W4" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="W4" s="4" t="s">
+      <c r="X4" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="X4" s="4" t="s">
+      <c r="Y4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="Y4" s="4" t="s">
+      <c r="Z4" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="Z4" s="4" t="s">
+      <c r="AA4" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC4" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD4" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="AE4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG4" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="AA4" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="AB4" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC4" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="AD4" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE4" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG4" s="4" t="s">
+      <c r="AH4" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="AH4" s="4" t="s">
+      <c r="AI4" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="AI4" s="4" t="s">
+      <c r="AJ4" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="AJ4" s="4" t="s">
+      <c r="AK4" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="AK4" s="4" t="s">
+      <c r="AL4" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="AL4" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="AM4" s="4" t="s">
         <v>124</v>
       </c>
       <c r="AN4" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AO4" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="AO4" s="4" t="s">
+      <c r="AP4" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="AP4" s="4" t="s">
+      <c r="AQ4" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="AQ4" s="4" t="s">
+      <c r="AR4" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AT4" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AU4" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="AR4" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="AS4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AT4" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="AU4" s="4" t="s">
-        <v>82</v>
-      </c>
       <c r="AV4" s="4" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="AW4" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="AX4" s="4"/>
+        <v>113</v>
+      </c>
+      <c r="AX4" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="AY4" s="4"/>
       <c r="AZ4" s="4" t="s">
         <v>9</v>
@@ -1519,184 +1471,72 @@
         <v>9</v>
       </c>
       <c r="BB4" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="BC4" s="6" t="s">
-        <v>12</v>
+        <v>114</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>9</v>
       </c>
       <c r="BD4" s="2"/>
     </row>
     <row r="5" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>135</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="R5" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="S5" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="T5" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="U5" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="V5" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="W5" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="X5" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y5" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z5" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA5" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="AB5" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC5" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="AD5" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="AE5" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF5" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG5" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH5" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AI5" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="AJ5" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="AK5" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="AL5" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AM5" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="AN5" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="AO5" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="AP5" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AQ5" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="AR5" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="AS5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AT5" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="AU5" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="AV5" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="AW5" s="4" t="s">
-        <v>134</v>
-      </c>
+      <c r="B5" s="1"/>
+      <c r="F5" s="2"/>
+      <c r="H5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="4"/>
+      <c r="AC5" s="4"/>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="4"/>
+      <c r="AG5" s="4"/>
+      <c r="AH5" s="4"/>
+      <c r="AI5" s="4"/>
+      <c r="AJ5" s="4"/>
+      <c r="AK5" s="4"/>
+      <c r="AL5" s="4"/>
+      <c r="AM5" s="4"/>
+      <c r="AN5" s="4"/>
+      <c r="AO5" s="4"/>
+      <c r="AP5" s="4"/>
+      <c r="AQ5" s="4"/>
+      <c r="AR5" s="4"/>
+      <c r="AS5" s="4"/>
+      <c r="AT5" s="7"/>
+      <c r="AU5" s="4"/>
+      <c r="AV5" s="4"/>
+      <c r="AW5" s="4"/>
       <c r="AX5" s="4"/>
       <c r="AY5" s="4"/>
-      <c r="AZ5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="BA5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="BB5" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="BC5" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="AZ5" s="4"/>
+      <c r="BA5" s="4"/>
+      <c r="BB5" s="4"/>
+      <c r="BC5" s="6"/>
       <c r="BD5" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="S2" r:id="rId1" display="d@gmail.com"/>
-    <hyperlink ref="S3:S5" r:id="rId2" display="d@gmail.com"/>
+    <hyperlink ref="S3" r:id="rId2" display="d@gmail.com"/>
     <hyperlink ref="B3" r:id="rId3"/>
-    <hyperlink ref="B4" r:id="rId4"/>
-    <hyperlink ref="B5" r:id="rId5"/>
+    <hyperlink ref="S4" r:id="rId4" display="d@gmail.com"/>
+    <hyperlink ref="B4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -1718,7 +1558,7 @@
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>